<commit_message>
SubRes_TRA_Techs: •	SubRes_TRA_Techs: added column Prc_Capact with 0.001 to all technologies •	In FI_Process table changed unit with Mpkm (Before it was Mpass-km) •	For PHEV reduced number of rows. For future years (2020 and 2035) only one row is enough to define the future cost VT_SHR_TRA_V01: •	Delated everything related to fuel blending (also commodity and process definition) •	From SEC_Comm changed description CO2 (delated “excluded aviation and navigation”
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_Techs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1365" windowWidth="17940" windowHeight="9855"/>
+    <workbookView xWindow="1452" yWindow="1368" windowWidth="17940" windowHeight="9852"/>
   </bookViews>
   <sheets>
     <sheet name="TRA_Passenger" sheetId="9" r:id="rId1"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0" shapeId="0">
+    <comment ref="B33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0">
+    <comment ref="F33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G35" authorId="0" shapeId="0">
+    <comment ref="G33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H35" authorId="0" shapeId="0">
+    <comment ref="H33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I35" authorId="0" shapeId="0">
+    <comment ref="I33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G42" authorId="0" shapeId="0">
+    <comment ref="G40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -475,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I42" authorId="0" shapeId="0">
+    <comment ref="I40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0">
+    <comment ref="B41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="93">
   <si>
     <t>~FI_T</t>
   </si>
@@ -972,9 +972,6 @@
     <t>MEUR2012</t>
   </si>
   <si>
-    <t>Mpass-km</t>
-  </si>
-  <si>
     <t>kvehicles</t>
   </si>
   <si>
@@ -1029,15 +1026,9 @@
     <t>TPCELC1N</t>
   </si>
   <si>
-    <t>Transport Passengers Car - Battery Electric Vehicle - Average battery size - New</t>
-  </si>
-  <si>
     <t>TPCGSLH1N</t>
   </si>
   <si>
-    <t>Transport Passengers Car -Hybrid Gasoline Engine -  Average size - New</t>
-  </si>
-  <si>
     <t>TPCELCH1N</t>
   </si>
   <si>
@@ -1047,18 +1038,34 @@
     <t>SHARE-I</t>
   </si>
   <si>
-    <t>Transport Passengers Car - Plug in hybrid Electric Vehicle  - Average size - New</t>
+    <t>PRC_CAPACT</t>
+  </si>
+  <si>
+    <t>Capacity to Activity Factor</t>
+  </si>
+  <si>
+    <t>Mpkm</t>
+  </si>
+  <si>
+    <t>Transport Passengers Car -Hybrid Gasoline Engine - New</t>
+  </si>
+  <si>
+    <t>Transport Passengers Car - Battery Electric Vehicle - New</t>
+  </si>
+  <si>
+    <t>Transport Passengers Car - Plug-in Hybrid Electric Vehicle - New</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
-    <numFmt numFmtId="187" formatCode="0.0"/>
-    <numFmt numFmtId="195" formatCode="0.00000"/>
-    <numFmt numFmtId="205" formatCode="0.000000"/>
-    <numFmt numFmtId="207" formatCode="\Te\x\t"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1189,7 +1196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1237,14 +1244,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1287,38 +1304,48 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="195" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="195" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="205" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="207" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="207" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="207" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="207" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="207" fontId="3" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="207" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="207" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="207" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1"/>
     <cellStyle name="Normal 10 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="4"/>
     <cellStyle name="Normale_B2020" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1756,48 +1783,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R57"/>
+  <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="53.21875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" customWidth="1"/>
-    <col min="18" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" customWidth="1"/>
+    <col min="18" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B2" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="15"/>
     </row>
-    <row r="4" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -1805,7 +1832,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>48</v>
       </c>
@@ -1818,7 +1845,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1844,10 +1871,10 @@
         <v>15</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>55</v>
@@ -1855,17 +1882,20 @@
       <c r="M7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="47" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
         <v>56</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" s="3" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="3" customFormat="1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>40</v>
       </c>
@@ -1907,12 +1937,14 @@
         <v>43</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q8"/>
+        <v>73</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="R8"/>
     </row>
-    <row r="9" spans="2:18" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" s="3" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>50</v>
       </c>
@@ -1925,31 +1957,31 @@
         <v>54</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K9" s="17"/>
       <c r="L9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="N9" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="O9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9"/>
+      <c r="Q9" s="17"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>LEFT(E10,4)&amp;RIGHT(D10,3)&amp;"1N"</f>
         <v>TPCDSL1N</v>
@@ -1972,7 +2004,7 @@
       <c r="H10" s="6">
         <v>2015</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="45">
         <v>296</v>
       </c>
       <c r="J10" s="6"/>
@@ -1992,8 +2024,11 @@
       <c r="P10" s="19">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q10" s="11">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -2007,7 +2042,7 @@
         <v>64</v>
       </c>
       <c r="H11" s="20"/>
-      <c r="I11" s="21">
+      <c r="I11" s="25">
         <f>I10*1.05</f>
         <v>310.8</v>
       </c>
@@ -2018,8 +2053,9 @@
       <c r="N11" s="20"/>
       <c r="O11" s="23"/>
       <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -2033,7 +2069,7 @@
         <v>64</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" s="21">
+      <c r="I12" s="25">
         <f>I11*1.05</f>
         <v>326.34000000000003</v>
       </c>
@@ -2044,17 +2080,18 @@
       <c r="N12" s="20"/>
       <c r="O12" s="23"/>
       <c r="P12" s="21"/>
-    </row>
-    <row r="13" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q12" s="43"/>
+    </row>
+    <row r="13" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="str">
         <f>LEFT(E13,4)&amp;RIGHT(D13,3)&amp;"1N"</f>
         <v>TPCGSL1N</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>63</v>
@@ -2068,7 +2105,7 @@
       <c r="H13" s="6">
         <v>2015</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="45">
         <v>391.7</v>
       </c>
       <c r="J13" s="6"/>
@@ -2088,8 +2125,11 @@
       <c r="P13" s="21">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q13" s="43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2103,7 +2143,7 @@
         <v>64</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="19">
+      <c r="I14" s="45">
         <f>I13*1.05</f>
         <v>411.28500000000003</v>
       </c>
@@ -2117,8 +2157,9 @@
       <c r="N14" s="20"/>
       <c r="O14" s="23"/>
       <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q14" s="43"/>
+    </row>
+    <row r="15" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2132,7 +2173,7 @@
         <v>64</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="19">
+      <c r="I15" s="45">
         <f>I14*1.05</f>
         <v>431.84925000000004</v>
       </c>
@@ -2146,20 +2187,21 @@
       <c r="N15" s="20"/>
       <c r="O15" s="23"/>
       <c r="P15" s="21"/>
-    </row>
-    <row r="16" spans="2:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q15" s="44"/>
+    </row>
+    <row r="16" spans="2:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="str">
         <f>LEFT(E16,3)&amp;RIGHT(D16,3)&amp;"1N"</f>
         <v>TPRELC1N</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>81</v>
       </c>
       <c r="F16" s="26">
         <v>2015</v>
@@ -2170,7 +2212,7 @@
       <c r="H16" s="26">
         <v>2015</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="46">
         <v>28.1</v>
       </c>
       <c r="J16" s="26"/>
@@ -2178,7 +2220,7 @@
       <c r="L16" s="26">
         <v>30</v>
       </c>
-      <c r="M16" s="27">
+      <c r="M16" s="46">
         <v>7155</v>
       </c>
       <c r="N16" s="28">
@@ -2190,13 +2232,16 @@
       <c r="P16" s="27">
         <v>74.358394573205203</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q16" s="43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="20">
         <v>2020</v>
@@ -2205,7 +2250,7 @@
         <v>64</v>
       </c>
       <c r="H17" s="20"/>
-      <c r="I17" s="21">
+      <c r="I17" s="25">
         <f>1.04*I16</f>
         <v>29.224000000000004</v>
       </c>
@@ -2216,13 +2261,14 @@
       <c r="N17" s="24"/>
       <c r="O17" s="20"/>
       <c r="P17" s="21"/>
-    </row>
-    <row r="18" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q17" s="43"/>
+    </row>
+    <row r="18" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="20">
         <v>2035</v>
@@ -2231,7 +2277,7 @@
         <v>64</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" s="21">
+      <c r="I18" s="25">
         <f>1.16*I16</f>
         <v>32.595999999999997</v>
       </c>
@@ -2242,16 +2288,17 @@
       <c r="N18" s="24"/>
       <c r="O18" s="20"/>
       <c r="P18" s="21"/>
-    </row>
-    <row r="19" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q18" s="43"/>
+    </row>
+    <row r="19" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>63</v>
@@ -2265,7 +2312,7 @@
       <c r="H19" s="29">
         <v>2015</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="30">
         <f>I13*1.4</f>
         <v>548.38</v>
       </c>
@@ -2288,8 +2335,11 @@
       <c r="P19" s="29">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q19" s="43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
@@ -2303,7 +2353,7 @@
         <v>64</v>
       </c>
       <c r="H20" s="29"/>
-      <c r="I20" s="32">
+      <c r="I20" s="30">
         <f>I19*1.02</f>
         <v>559.34760000000006</v>
       </c>
@@ -2319,8 +2369,9 @@
       <c r="N20" s="29"/>
       <c r="O20" s="29"/>
       <c r="P20" s="29"/>
-    </row>
-    <row r="21" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q20" s="43"/>
+    </row>
+    <row r="21" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2334,7 +2385,7 @@
         <v>64</v>
       </c>
       <c r="H21" s="29"/>
-      <c r="I21" s="32">
+      <c r="I21" s="30">
         <f>I20*1.05</f>
         <v>587.31498000000011</v>
       </c>
@@ -2350,16 +2401,17 @@
       <c r="N21" s="29"/>
       <c r="O21" s="29"/>
       <c r="P21" s="29"/>
-    </row>
-    <row r="22" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q21" s="43"/>
+    </row>
+    <row r="22" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>63</v>
@@ -2373,7 +2425,7 @@
       <c r="H22" s="29">
         <v>2015</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="30">
         <v>1388.9</v>
       </c>
       <c r="J22" s="29"/>
@@ -2394,8 +2446,11 @@
       <c r="P22" s="29">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q22" s="43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
@@ -2425,8 +2480,9 @@
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
       <c r="P23" s="29"/>
-    </row>
-    <row r="24" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q23" s="43"/>
+    </row>
+    <row r="24" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
@@ -2440,7 +2496,7 @@
         <v>64</v>
       </c>
       <c r="H24" s="29"/>
-      <c r="I24" s="32">
+      <c r="I24" s="30">
         <f>I23*1.07</f>
         <v>1560.4291500000004</v>
       </c>
@@ -2456,16 +2512,17 @@
       <c r="N24" s="29"/>
       <c r="O24" s="29"/>
       <c r="P24" s="29"/>
-    </row>
-    <row r="25" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q24" s="43"/>
+    </row>
+    <row r="25" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>63</v>
@@ -2493,7 +2550,7 @@
         <f>222122.65452346*0.135/1000</f>
         <v>29.986558360667104</v>
       </c>
-      <c r="N25" s="33">
+      <c r="N25" s="32">
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="O25" s="29">
@@ -2502,12 +2559,15 @@
       <c r="P25" s="29">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q25" s="43">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>63</v>
@@ -2520,7 +2580,7 @@
       </c>
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
-      <c r="J26" s="29">
+      <c r="J26" s="30">
         <v>392.98999999999995</v>
       </c>
       <c r="K26" s="29">
@@ -2531,8 +2591,9 @@
       <c r="N26" s="29"/>
       <c r="O26" s="29"/>
       <c r="P26" s="29"/>
-    </row>
-    <row r="27" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q26" s="43"/>
+    </row>
+    <row r="27" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -2557,8 +2618,9 @@
       <c r="N27" s="29"/>
       <c r="O27" s="29"/>
       <c r="P27" s="29"/>
-    </row>
-    <row r="28" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q27" s="43"/>
+    </row>
+    <row r="28" spans="2:17" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
@@ -2566,7 +2628,7 @@
         <v>63</v>
       </c>
       <c r="F28" s="29">
-        <v>2020</v>
+        <v>2035</v>
       </c>
       <c r="G28" s="29" t="s">
         <v>64</v>
@@ -2576,369 +2638,324 @@
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
       <c r="L28" s="29"/>
-      <c r="M28" s="30"/>
+      <c r="M28" s="30">
+        <f>0.9*M27</f>
+        <v>23.749354221648346</v>
+      </c>
       <c r="N28" s="29"/>
       <c r="O28" s="29"/>
       <c r="P28" s="29"/>
-    </row>
-    <row r="29" spans="2:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="29">
-        <v>2035</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="30">
-        <f>0.9*M27</f>
-        <v>23.749354221648346</v>
-      </c>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="29">
-        <v>2035</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="34" t="s">
+      <c r="Q28" s="43"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="36" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D33" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="37" t="s">
+      <c r="E33" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F33" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G33" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H33" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="37" t="s">
+      <c r="I33" s="36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="38" t="s">
+    <row r="34" spans="2:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C34" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D34" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="38" t="s">
+      <c r="E34" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F34" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="38" t="s">
+      <c r="G34" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="38" t="s">
+      <c r="H34" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="38" t="s">
+      <c r="I34" s="37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="34" t="s">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="40" t="s">
+      <c r="C39" s="33"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C40" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D40" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E40" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F40" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="40" t="s">
+      <c r="G40" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H42" s="40" t="s">
+      <c r="H40" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I40" s="39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="41" t="s">
+    <row r="41" spans="2:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C41" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="41" t="s">
+      <c r="D41" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="41" t="s">
+      <c r="E41" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="41" t="s">
+      <c r="F41" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="G43" s="41" t="s">
+      <c r="G41" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="H43" s="41" t="s">
+      <c r="H41" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I43" s="41" t="s">
+      <c r="I41" s="40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="42" t="str">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="41" t="str">
         <f>B10</f>
         <v>TPCDSL1N</v>
       </c>
-      <c r="D44" s="42" t="str">
+      <c r="D42" s="41" t="str">
         <f>C10</f>
         <v>Transport Passengers Car - Diesel Engine - New</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E42" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" s="42" t="s">
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42" t="str">
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41" t="str">
         <f>B16</f>
         <v>TPRELC1N</v>
       </c>
-      <c r="D46" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="42" t="s">
+      <c r="D44" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F46" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="42"/>
-      <c r="C47" s="42" t="str">
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41" t="str">
         <f>B19</f>
         <v>TPCGSLH1N</v>
       </c>
-      <c r="D47" s="42" t="str">
+      <c r="D45" s="41" t="str">
         <f>C19</f>
-        <v>Transport Passengers Car -Hybrid Gasoline Engine -  Average size - New</v>
-      </c>
-      <c r="E47" s="42" t="s">
+        <v>Transport Passengers Car -Hybrid Gasoline Engine - New</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="42"/>
-      <c r="C48" s="42" t="str">
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41" t="str">
         <f>B22</f>
         <v>TPCELC1N</v>
       </c>
-      <c r="D48" s="42" t="str">
+      <c r="D46" s="41" t="str">
         <f>C22</f>
-        <v>Transport Passengers Car - Battery Electric Vehicle - Average battery size - New</v>
-      </c>
-      <c r="E48" s="42" t="s">
+        <v>Transport Passengers Car - Battery Electric Vehicle - New</v>
+      </c>
+      <c r="E46" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F48" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42" t="str">
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41" t="str">
         <f>B25</f>
         <v>TPCELCH1N</v>
       </c>
-      <c r="D49" s="42" t="str">
+      <c r="D47" s="41" t="str">
         <f>C25</f>
-        <v>Transport Passengers Car - Plug in hybrid Electric Vehicle  - Average size - New</v>
-      </c>
-      <c r="E49" s="42" t="s">
+        <v>Transport Passengers Car - Plug-in Hybrid Electric Vehicle - New</v>
+      </c>
+      <c r="E47" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="8" t="s">
+      <c r="C50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="10" t="s">
+    <row r="52" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>